<commit_message>
EPBDS-8874 Fix error. Use full refference name to the spreadsheet cell instead of simple introduced in 5.23
--HG--
branch : 5.22.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/expected-test-failures/EPBDS-8874_Method_Dispatching.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/expected-test-failures/EPBDS-8874_Method_Dispatching.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
   <si>
     <t>Spreadsheet SpreadsheetResult someCalculation(Integer a)</t>
   </si>
@@ -102,30 +102,23 @@
     <t>Somevalues</t>
   </si>
   <si>
-    <t>_res_</t>
-  </si>
-  <si>
     <t>Result</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>_res_.$Step1</t>
-  </si>
-  <si>
-    <t>_res_.$Step2</t>
+    <t>_res_.$Values$Step2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -139,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -178,28 +171,25 @@
       <diagonal/>
     </border>
     <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -208,8 +198,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,13 +532,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22:J28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="2" max="2" width="20" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -572,11 +564,11 @@
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
@@ -614,11 +606,11 @@
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
@@ -656,14 +648,14 @@
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
@@ -716,11 +708,11 @@
       <c r="I27" s="7"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
@@ -806,42 +798,42 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44">
-      <c r="B44" s="9" t="s">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="9"/>
-    </row>
-    <row r="45">
-      <c r="B45" t="s" s="9">
+      <c r="C44" s="10"/>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C45" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="B46" t="s" s="9">
+      <c r="C45" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C46" t="s" s="9">
+      <c r="C46" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="8"/>
+      <c r="C47" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="47">
-      <c r="B47" s="9"/>
-      <c r="C47" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B44:C44"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="G23:I23"/>
-    <mergeCell ref="B44:C44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>